<commit_message>
modifications for Power BI implementation
</commit_message>
<xml_diff>
--- a/data/Input 2 - School Data.xlsx
+++ b/data/Input 2 - School Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLuedtke\ACM-School-Placement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLuedtke\ACM-School-Placement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Input - School Parameters" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Input - School Parameters'!$A$1:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Input - School Parameters'!$A$1:$G$27</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Team Size</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>7:11AM</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
@@ -614,672 +620,679 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <f ca="1">RANDBETWEEN(0, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="D3">
-        <v>9</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
         <v>3.5</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F27" ca="1" si="0">RANDBETWEEN(0, 2)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3">
+        <f t="shared" ref="H3:H27" ca="1" si="0">RANDBETWEEN(0, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
         <v>43.1</v>
       </c>
-      <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
         <v>3.2</v>
       </c>
-      <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
         <v>0.9</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <v>0.3</v>
       </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
         <v>4.2</v>
       </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>1.6</v>
       </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
         <v>1.6</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>67</v>
       </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
         <v>0.8</v>
       </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>65</v>
       </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
         <v>55.7</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
-      </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13">
         <v>1.5</v>
       </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14">
-        <v>9</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
         <v>2.6</v>
       </c>
-      <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>10.3</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
         <v>1.9</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>66</v>
       </c>
-      <c r="D17">
-        <v>9</v>
-      </c>
-      <c r="E17">
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
         <v>90.2</v>
       </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18">
-        <v>9</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
         <v>1.8</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19">
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>63.6</v>
       </c>
-      <c r="F19">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20">
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20">
         <v>10</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>11.5</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21">
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21">
         <v>10</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>66</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>10</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>2.9</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23">
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23">
         <v>11</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>1.4</v>
       </c>
-      <c r="F23">
+      <c r="H23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>79</v>
+      </c>
+      <c r="H24">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24">
-        <v>11</v>
-      </c>
-      <c r="E24">
-        <v>79</v>
-      </c>
-      <c r="F24">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>56</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>65</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>11</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>38</v>
       </c>
-      <c r="F25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="H25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26">
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26">
         <v>11</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>5.9</v>
       </c>
-      <c r="F26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>65</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>11</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>0.9</v>
       </c>
-      <c r="F27">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E27"/>
+  <autoFilter ref="A1:G27"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>